<commit_message>
commit mutilanguage cho HOme
</commit_message>
<xml_diff>
--- a/docs/Sprint 5 - 1904 To 0305/LogTime.xlsx
+++ b/docs/Sprint 5 - 1904 To 0305/LogTime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ANLT" sheetId="1" r:id="rId1"/>
@@ -20,91 +20,106 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>4/7/2014</t>
-  </si>
-  <si>
-    <t>4/8/2014</t>
-  </si>
-  <si>
-    <t>4/9/2014</t>
-  </si>
-  <si>
-    <t>4/10/2014</t>
-  </si>
-  <si>
-    <t>4/11/2014</t>
-  </si>
-  <si>
-    <t>4/12/2014</t>
-  </si>
-  <si>
-    <t>4/13/2014</t>
-  </si>
-  <si>
-    <t>4/14/2014</t>
-  </si>
-  <si>
-    <t>4/15/2014</t>
-  </si>
-  <si>
-    <t>4/16/2014</t>
-  </si>
-  <si>
-    <t>4/17/2014</t>
-  </si>
-  <si>
-    <t>4/18/2014</t>
-  </si>
-  <si>
-    <t>4/19/2014</t>
-  </si>
-  <si>
-    <t>4/20/2014</t>
-  </si>
-  <si>
-    <t>Payment - Database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payment - model </t>
-  </si>
-  <si>
-    <t>Refactor : model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin Login page </t>
-  </si>
-  <si>
-    <t xml:space="preserve">và cơ chế phân biệt giữa user và admin </t>
-  </si>
-  <si>
-    <t>Update login subsystem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metting + Quản lý team task </t>
-  </si>
-  <si>
-    <t>Hoàn thành PIN, có thể pin từ product/details/1. trong pin ta có thể làm movetocart, movetowishlist, remove mà không cần load lại trang</t>
-  </si>
-  <si>
-    <t>Chat</t>
+    <t>21/04/2014</t>
+  </si>
+  <si>
+    <t>22/04/2014</t>
+  </si>
+  <si>
+    <t>23/04/2014</t>
+  </si>
+  <si>
+    <t>24/04/2014</t>
+  </si>
+  <si>
+    <t>25/04/2014</t>
+  </si>
+  <si>
+    <t>26/04/2014</t>
+  </si>
+  <si>
+    <t>27/04/2014</t>
+  </si>
+  <si>
+    <t>28/04/2014</t>
+  </si>
+  <si>
+    <t>29/04/2014</t>
+  </si>
+  <si>
+    <t>30/04/2014</t>
+  </si>
+  <si>
+    <t>01/05/2014</t>
+  </si>
+  <si>
+    <t>02/05/2014</t>
+  </si>
+  <si>
+    <t>03/05/2014</t>
+  </si>
+  <si>
+    <t>04/05/2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cắt HTML -home </t>
+  </si>
+  <si>
+    <t>thêm angular js vs bootstraps cho mockup</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> update giao diện cho portal. - login, change password.</t>
+  </si>
+  <si>
+    <t>Meeting + thay đổi giao diện user</t>
+  </si>
+  <si>
+    <t>UPdate giao diện cho phần account</t>
+  </si>
+  <si>
+    <t>User Account</t>
+  </si>
+  <si>
+    <t>order history</t>
+  </si>
+  <si>
+    <t>Ghép giao diện phần order history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đa ngôn ngữ cho các màn đã làm. </t>
+  </si>
+  <si>
+    <t>Cắt giao diện màn hình details.</t>
+  </si>
+  <si>
+    <t>Home Menu, Hot, tất cả đều Ajax</t>
+  </si>
+  <si>
+    <t>Trang chủ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF141823"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,22 +142,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -158,51 +174,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:O10" totalsRowCount="1" headerRowDxfId="1">
-  <autoFilter ref="A1:O10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:O13" totalsRowCount="1" headerRowDxfId="1">
+  <autoFilter ref="A1:O12"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="4/7/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/7/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="3" name="4/8/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/8/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="4" name="4/9/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/9/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="5" name="4/10/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/10/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="6" name="4/11/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/11/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="7" name="4/12/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/12/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="8" name="4/13/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/13/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="9" name="4/14/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/14/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="10" name="4/15/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/15/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="11" name="4/16/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/16/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="12" name="4/17/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/17/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="13" name="4/18/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/18/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="14" name="4/19/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/19/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="15" name="4/20/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table2[4/20/2014])</totalsRowFormula>
+    <tableColumn id="1" name="order history"/>
+    <tableColumn id="2" name="21/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[21/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" name="22/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[22/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" name="23/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[23/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" name="24/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[24/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="25/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[25/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" name="26/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[26/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" name="27/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[27/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="9" name="28/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[28/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="10" name="29/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[29/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="11" name="30/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[30/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="12" name="01/05/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[01/05/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="13" name="02/05/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[02/05/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="14" name="03/05/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[03/05/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="15" name="04/05/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table2[04/05/2014])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -214,47 +230,47 @@
   <autoFilter ref="A1:O9"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="4/7/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/7/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="3" name="4/8/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/8/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="4" name="4/9/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/9/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="5" name="4/10/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/10/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="6" name="4/11/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/11/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="7" name="4/12/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/12/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="8" name="4/13/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/13/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="9" name="4/14/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/14/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="10" name="4/15/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/15/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="11" name="4/16/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/16/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="12" name="4/17/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/17/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="13" name="4/18/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/18/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="14" name="4/19/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/19/2014])</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="15" name="4/20/2014" totalsRowFunction="custom">
-      <totalsRowFormula>SUM(Table24[4/20/2014])</totalsRowFormula>
+    <tableColumn id="2" name="21/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[21/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" name="22/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[22/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" name="23/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[23/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" name="24/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[24/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="25/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[25/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" name="26/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[26/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" name="27/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[27/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="9" name="28/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[28/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="10" name="29/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[29/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="11" name="30/04/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[30/04/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="12" name="01/05/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[01/05/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="13" name="02/05/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[02/05/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="14" name="03/05/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[03/05/2014])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="15" name="04/05/2014" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table24[04/05/2014])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -524,15 +540,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="49" customWidth="1"/>
     <col min="2" max="13" width="13" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" customWidth="1"/>
     <col min="15" max="15" width="12.140625" customWidth="1"/>
@@ -542,8 +558,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -593,32 +609,26 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -626,98 +636,118 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
+        <v>19</v>
+      </c>
+      <c r="G6">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8">
+        <v>22</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <f>SUM(Table2[4/7/2014])</f>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f>SUM(Table2[21/04/2014])</f>
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <f>SUM(Table2[22/04/2014])</f>
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <f>SUM(Table2[23/04/2014])</f>
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <f>SUM(Table2[24/04/2014])</f>
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f>SUM(Table2[25/04/2014])</f>
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <f>SUM(Table2[26/04/2014])</f>
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <f>SUM(Table2[27/04/2014])</f>
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <f>SUM(Table2[28/04/2014])</f>
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <f>SUM(Table2[29/04/2014])</f>
+        <v>6</v>
+      </c>
+      <c r="K13">
+        <f>SUM(Table2[30/04/2014])</f>
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <f>SUM(Table2[01/05/2014])</f>
         <v>3</v>
       </c>
-      <c r="C10">
-        <f>SUM(Table2[4/8/2014])</f>
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <f>SUM(Table2[4/9/2014])</f>
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <f>SUM(Table2[4/10/2014])</f>
-        <v>4</v>
-      </c>
-      <c r="F10">
-        <f>SUM(Table2[4/11/2014])</f>
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <f>SUM(Table2[4/12/2014])</f>
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <f>SUM(Table2[4/13/2014])</f>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f>SUM(Table2[4/14/2014])</f>
-        <v>4</v>
-      </c>
-      <c r="J10">
-        <f>SUM(Table2[4/15/2014])</f>
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <f>SUM(Table2[4/16/2014])</f>
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <f>SUM(Table2[4/17/2014])</f>
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <f>SUM(Table2[4/18/2014])</f>
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <f>SUM(Table2[4/19/2014])</f>
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <f>SUM(Table2[4/20/2014])</f>
+      <c r="M13">
+        <f>SUM(Table2[02/05/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f>SUM(Table2[03/05/2014])</f>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>SUM(Table2[04/05/2014])</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -726,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,77 +816,77 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="F2">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10">
-        <f>SUM(Table24[4/7/2014])</f>
+        <f>SUM(Table24[21/04/2014])</f>
         <v>0</v>
       </c>
       <c r="C10">
-        <f>SUM(Table24[4/8/2014])</f>
-        <v>4</v>
+        <f>SUM(Table24[22/04/2014])</f>
+        <v>0</v>
       </c>
       <c r="D10">
-        <f>SUM(Table24[4/9/2014])</f>
+        <f>SUM(Table24[23/04/2014])</f>
         <v>0</v>
       </c>
       <c r="E10">
-        <f>SUM(Table24[4/10/2014])</f>
+        <f>SUM(Table24[24/04/2014])</f>
         <v>0</v>
       </c>
       <c r="F10">
-        <f>SUM(Table24[4/11/2014])</f>
-        <v>0</v>
+        <f>SUM(Table24[25/04/2014])</f>
+        <v>4</v>
       </c>
       <c r="G10">
-        <f>SUM(Table24[4/12/2014])</f>
+        <f>SUM(Table24[26/04/2014])</f>
         <v>0</v>
       </c>
       <c r="H10">
-        <f>SUM(Table24[4/13/2014])</f>
-        <v>0</v>
+        <f>SUM(Table24[27/04/2014])</f>
+        <v>4</v>
       </c>
       <c r="I10">
-        <f>SUM(Table24[4/14/2014])</f>
-        <v>8</v>
+        <f>SUM(Table24[28/04/2014])</f>
+        <v>0</v>
       </c>
       <c r="J10">
-        <f>SUM(Table24[4/15/2014])</f>
+        <f>SUM(Table24[29/04/2014])</f>
         <v>0</v>
       </c>
       <c r="K10">
-        <f>SUM(Table24[4/16/2014])</f>
+        <f>SUM(Table24[30/04/2014])</f>
         <v>0</v>
       </c>
       <c r="L10">
-        <f>SUM(Table24[4/17/2014])</f>
+        <f>SUM(Table24[01/05/2014])</f>
         <v>0</v>
       </c>
       <c r="M10">
-        <f>SUM(Table24[4/18/2014])</f>
+        <f>SUM(Table24[02/05/2014])</f>
         <v>0</v>
       </c>
       <c r="N10">
-        <f>SUM(Table24[4/19/2014])</f>
+        <f>SUM(Table24[03/05/2014])</f>
         <v>0</v>
       </c>
       <c r="O10">
-        <f>SUM(Table24[4/20/2014])</f>
+        <f>SUM(Table24[04/05/2014])</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit log time, 2 màn hình : lựa chọn phương thức thanh toán, order review. Thanh toán ngân lượng
</commit_message>
<xml_diff>
--- a/docs/Sprint 5 - 1904 To 0305/LogTime.xlsx
+++ b/docs/Sprint 5 - 1904 To 0305/LogTime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165"/>
   </bookViews>
   <sheets>
     <sheet name="ANLT" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>Trang chủ</t>
+  </si>
+  <si>
+    <t>Update cơ chế phần đa ngôn ngữ cho sub và update ngôn ngữ trên home</t>
+  </si>
+  <si>
+    <t>Details chưa có rating &amp; review do đã thống nhất chưa làm. Hiện tại đã có thể bấm vào add to cart và add to wishlist</t>
+  </si>
+  <si>
+    <t>Metting</t>
+  </si>
+  <si>
+    <t>Metting + Support(Time và task dự án)</t>
   </si>
 </sst>
 </file>
@@ -542,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,6 +697,25 @@
         <v>3</v>
       </c>
     </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+    </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>SUM(Table2[21/04/2014])</f>
@@ -732,7 +763,7 @@
       </c>
       <c r="M13">
         <f>SUM(Table2[02/05/2014])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N13">
         <f>SUM(Table2[03/05/2014])</f>
@@ -740,7 +771,7 @@
       </c>
       <c r="O13">
         <f>SUM(Table2[04/05/2014])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -756,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,6 +863,22 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+    </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>SUM(Table24[21/04/2014])</f>
@@ -883,11 +930,11 @@
       </c>
       <c r="N10">
         <f>SUM(Table24[03/05/2014])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O10">
         <f>SUM(Table24[04/05/2014])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>